<commit_message>
MAE 64 and MAPE 67%
</commit_message>
<xml_diff>
--- a/datasets_resumidos/resumen_cupos_2021A.xlsx
+++ b/datasets_resumidos/resumen_cupos_2021A.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -570,480 +570,432 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>COMPUTO FLEXIBLE (SOFTCOMPUTING)</t>
+          <t>CONTROL DE PROYECTOS</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>99</v>
+        <v>271</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D9" t="n">
-        <v>39</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CONTROL DE PROYECTOS</t>
+          <t>ESTADISTICA Y PROCESOS ESTOCASTICOS</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>271</v>
+        <v>643</v>
       </c>
       <c r="C10" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D10" t="n">
-        <v>116</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ESTADISTICA Y PROCESOS ESTOCASTICOS</t>
+          <t>ESTRUCTURAS DE DATOS I</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>643</v>
+        <v>721</v>
       </c>
       <c r="C11" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D11" t="n">
-        <v>31</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ESTRUCTURAS DE DATOS I</t>
+          <t>ESTRUCTURAS DE DATOS II</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>721</v>
+        <v>467</v>
       </c>
       <c r="C12" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>208</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ESTRUCTURAS DE DATOS II</t>
+          <t>HIPERMEDIA</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>467</v>
+        <v>280</v>
       </c>
       <c r="C13" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D13" t="n">
-        <v>131</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>HIPERMEDIA</t>
+          <t>INGENIERIA DE SOFTWARE I</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>280</v>
+        <v>385</v>
       </c>
       <c r="C14" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D14" t="n">
-        <v>61</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>INGENIERIA DE SOFTWARE I</t>
+          <t>INGENIERIA DE SOFTWARE II</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>385</v>
+        <v>160</v>
       </c>
       <c r="C15" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D15" t="n">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>INGENIERIA DE SOFTWARE II</t>
+          <t>MATEMATICA DISCRETA</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>160</v>
+        <v>608</v>
       </c>
       <c r="C16" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>MATEMATICA DISCRETA</t>
+          <t>METODOS MATEMATICOS I</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>608</v>
+        <v>1126</v>
       </c>
       <c r="C17" t="n">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="D17" t="n">
-        <v>50</v>
+        <v>256</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>METODOS MATEMATICOS I</t>
+          <t>METODOS MATEMATICOS II</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1126</v>
+        <v>926</v>
       </c>
       <c r="C18" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D18" t="n">
-        <v>256</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>METODOS MATEMATICOS II</t>
+          <t>MINERIA DE DATOS</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>926</v>
+        <v>160</v>
       </c>
       <c r="C19" t="n">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="D19" t="n">
-        <v>117</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>MINERIA DE DATOS</t>
+          <t>PROGRAMACION</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>160</v>
+        <v>1402</v>
       </c>
       <c r="C20" t="n">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="D20" t="n">
-        <v>45</v>
+        <v>528</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>PROGRAMACION</t>
+          <t>PROGRAMACION PARA INTERNET</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1402</v>
+        <v>640</v>
       </c>
       <c r="C21" t="n">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="D21" t="n">
-        <v>528</v>
+        <v>323</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>PROGRAMACION PARA INTERNET</t>
+          <t>SEGURIDAD DE LA INFORMACION</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>640</v>
+        <v>137</v>
       </c>
       <c r="C22" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="D22" t="n">
-        <v>323</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>PROYECTO DE GESTION DE LA TECNOLOGIA DE INFORMACION</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE BASES DE DATOS</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>99</v>
+        <v>380</v>
       </c>
       <c r="C23" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D23" t="n">
-        <v>41</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>PROYECTO DE SISTEMAS ROBUSTOS, PARALELOS Y DISTRIBUIDOS</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE PROGRAMACION</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>99</v>
+        <v>911</v>
       </c>
       <c r="C24" t="n">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="D24" t="n">
-        <v>42</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>SEGURIDAD DE LA INFORMACION</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE ALGORITMIA</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>137</v>
+        <v>420</v>
       </c>
       <c r="C25" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D25" t="n">
-        <v>7</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE BASES DE DATOS</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE ESTRUCTURAS DE DATOS I</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>380</v>
+        <v>552</v>
       </c>
       <c r="C26" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D26" t="n">
-        <v>16</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE PROGRAMACION</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE ESTRUCTURAS DE DATOS II</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>911</v>
+        <v>320</v>
       </c>
       <c r="C27" t="n">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="D27" t="n">
-        <v>53</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE ALGORITMIA</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE METODOS MATEMATICOS I</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>420</v>
+        <v>1240</v>
       </c>
       <c r="C28" t="n">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="D28" t="n">
-        <v>38</v>
+        <v>332</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE ESTRUCTURAS DE DATOS I</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE METODOS MATEMATICOS II</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>552</v>
+        <v>924</v>
       </c>
       <c r="C29" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D29" t="n">
-        <v>76</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE ESTRUCTURAS DE DATOS II</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE INGENIERIA DE SOFTWARE I</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>320</v>
+        <v>265</v>
       </c>
       <c r="C30" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D30" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE METODOS MATEMATICOS I</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE USO, ADAPTACION, EXPLOTACION DE SISTEMAS OPERATIVOS</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>1240</v>
+        <v>131</v>
       </c>
       <c r="C31" t="n">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="D31" t="n">
-        <v>332</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE METODOS MATEMATICOS II</t>
+          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE SISTEMAS BASADOS EN CONOCIMIENTO</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>924</v>
+        <v>125</v>
       </c>
       <c r="C32" t="n">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="D32" t="n">
-        <v>90</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE INGENIERIA DE SOFTWARE I</t>
+          <t>SISTEMAS BASADOS EN CONOCIMIENTO</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>265</v>
+        <v>125</v>
       </c>
       <c r="C33" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D33" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE USO, ADAPTACION, EXPLOTACION DE SISTEMAS OPERATIVOS</t>
+          <t>TEORIA DE LA COMPUTACION</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>131</v>
+        <v>401</v>
       </c>
       <c r="C34" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D34" t="n">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>SEMINARIO DE SOLUCION DE PROBLEMAS DE SISTEMAS BASADOS EN CONOCIMIENTO</t>
+          <t>USO, ADAPTACION Y EXPLOTACION DE SISTEMAS OPERATIVOS</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C35" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D35" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>SISTEMAS BASADOS EN CONOCIMIENTO</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>125</v>
-      </c>
-      <c r="C36" t="n">
-        <v>5</v>
-      </c>
-      <c r="D36" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>TEORIA DE LA COMPUTACION</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>401</v>
-      </c>
-      <c r="C37" t="n">
-        <v>10</v>
-      </c>
-      <c r="D37" t="n">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>USO, ADAPTACION Y EXPLOTACION DE SISTEMAS OPERATIVOS</t>
-        </is>
-      </c>
-      <c r="B38" t="n">
-        <v>120</v>
-      </c>
-      <c r="C38" t="n">
-        <v>3</v>
-      </c>
-      <c r="D38" t="n">
         <v>12</v>
       </c>
     </row>

</xml_diff>